<commit_message>
Error fixed but its ugly af
</commit_message>
<xml_diff>
--- a/Assignment 2/oo.xlsx
+++ b/Assignment 2/oo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Norman\PycharmProjects\3522_Assignment2_A01043914_A00893016\Assignment 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46FE603-CF27-4027-9F0F-9BDECF55BAC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC0C557-8114-44CE-9E35-C8945316F4A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="26730" windowHeight="11505" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="26730" windowHeight="14955" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
   <si>
     <t>name</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>deed</t>
+  </si>
+  <si>
+    <t>poasd</t>
+  </si>
+  <si>
+    <t>sdaasd</t>
   </si>
 </sst>
 </file>
@@ -669,9 +675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC969572-FB28-418E-B89D-F0DD002AE5AA}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,6 +1093,9 @@
       <c r="G10" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="K10">
+        <v>-9</v>
+      </c>
       <c r="Q10" t="s">
         <v>90</v>
       </c>
@@ -1119,6 +1128,9 @@
       <c r="G11" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="K11" t="s">
+        <v>94</v>
+      </c>
       <c r="Q11" t="s">
         <v>82</v>
       </c>
@@ -1161,7 +1173,7 @@
         <v>9</v>
       </c>
       <c r="L12">
-        <v>15</v>
+        <v>-89</v>
       </c>
       <c r="M12">
         <v>5</v>
@@ -1201,8 +1213,8 @@
       <c r="I13">
         <v>5</v>
       </c>
-      <c r="L13">
-        <v>4</v>
+      <c r="L13" t="s">
+        <v>95</v>
       </c>
       <c r="M13">
         <v>1</v>

</xml_diff>